<commit_message>
Apresentação Slides + Execuções GEO AGEO + Novas FOs + Diagrama tudo
</commit_message>
<xml_diff>
--- a/Resultados_GEO_SpacecraftOptimization/resultados_GEO_SPACE.xlsx
+++ b/Resultados_GEO_SpacecraftOptimization/resultados_GEO_SPACE.xlsx
@@ -13,34 +13,26 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>GEO</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -61,9 +53,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -77,15 +106,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -99,16 +137,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -129,46 +174,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,7 +191,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -195,13 +233,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -213,13 +335,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -231,139 +365,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -387,16 +395,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -417,36 +425,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -474,153 +462,173 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1025,45 +1033,36 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="false"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="false"/>
+    <c:autoTitleDeleted val="true"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.168841710896035"/>
+          <c:y val="0.0471698113207547"/>
+          <c:w val="0.807586637527318"/>
+          <c:h val="0.760377358490566"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="marker"/>
         <c:varyColors val="false"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GEO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -1072,15 +1071,13 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="x"/>
+            <c:size val="4"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1180,20 +1177,55 @@
         </c:scaling>
         <c:delete val="false"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr defTabSz="914400">
+                  <a:defRPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT" altLang="en-US" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>t</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-PT" altLang="en-US" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.544848579456759"/>
+              <c:y val="0.911878216123499"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="false"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="true"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1218,10 +1250,7 @@
             <a:pPr>
               <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1242,20 +1271,55 @@
         </c:scaling>
         <c:delete val="false"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr defTabSz="914400">
+                  <a:defRPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT" altLang="en-US" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>NFE</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-PT" altLang="en-US" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0173275054636278"/>
+              <c:y val="0.41438679245283"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="false"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="true"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1280,10 +1344,7 @@
             <a:pPr>
               <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1304,6 +1365,60 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.549304058027838"/>
+          <c:y val="0.128522336769759"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="false"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="true"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="false"/>
@@ -1328,7 +1443,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr lang="en-US"/>
+        <a:defRPr lang="en-US">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
     </a:p>
   </c:txPr>
@@ -2492,10 +2611,10 @@
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>438785</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>581660</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>151765</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2504,7 +2623,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3648075" y="3524250"/>
-        <a:ext cx="3239135" cy="2771775"/>
+        <a:ext cx="4067810" cy="2961640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2777,8 +2896,8 @@
   <sheetPr/>
   <dimension ref="C4:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="5"/>
@@ -2897,6 +3016,11 @@
         <v>2.5</v>
       </c>
     </row>
+    <row r="22" spans="4:4">
+      <c r="D22" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="23" spans="3:4">
       <c r="C23">
         <v>0.5</v>

</xml_diff>